<commit_message>
Can upload excel file and read data into pandas dataframe
</commit_message>
<xml_diff>
--- a/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
+++ b/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\617626\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3146C51D-945A-41BE-B761-481B0A59ADDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAFD446-3AC0-4963-BE6D-0223658254AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E7FB1D0-DDC4-4D5E-A804-8C26471E00FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>A1 Cell</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>This is just a test file, leave all sheet names as they are</t>
   </si>
 </sst>
 </file>
@@ -415,7 +419,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,4 +460,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF51519-8C4E-4ADE-9329-C30AF300D902}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
right about to make first data cleaning a function so it can be called in main in init.py. Things currently work in the emulator nlpinputs, but older versions of the file are getting referenced because I am using import* to get in data_clean. Basically learned that init goes off when the function gets launched one time, but main goes off on each trigger.
</commit_message>
<xml_diff>
--- a/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
+++ b/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\617626\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D5778-29DD-4AF1-85FC-4442DD2DBD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA14629F-1AE5-49BE-A94D-999B42E71674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{8E7FB1D0-DDC4-4D5E-A804-8C26471E00FA}"/>
   </bookViews>
@@ -67,7 +67,7 @@
     <t>This is just a test file, leave all sheet names as they are</t>
   </si>
   <si>
-    <t>Hey Dillen its eleven</t>
+    <t>Hey Dillen its two thirty</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
It might actually work right now. I made data_clean a return on a function. I am 99% sure that the emulator is only accepting file names that are also in the storage explorer (non emulator). I think init lines 26-29 are triggering and getting what was put into the emulator, and the rest of init is pointing to the non emulator nlpinputs
</commit_message>
<xml_diff>
--- a/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
+++ b/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\617626\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA14629F-1AE5-49BE-A94D-999B42E71674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D5778-29DD-4AF1-85FC-4442DD2DBD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{8E7FB1D0-DDC4-4D5E-A804-8C26471E00FA}"/>
   </bookViews>
@@ -67,7 +67,7 @@
     <t>This is just a test file, leave all sheet names as they are</t>
   </si>
   <si>
-    <t>Hey Dillen its two thirty</t>
+    <t>Hey Dillen its eleven</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
All done through SecondExploratoryDataAnalysis. Ready to start on sentiment analysis
</commit_message>
<xml_diff>
--- a/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
+++ b/BlobTrigger1/Data_Holder_Folder/FileyTheFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\617626\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D5778-29DD-4AF1-85FC-4442DD2DBD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F5B181-78CE-4944-9485-4CA9D2D1AFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{8E7FB1D0-DDC4-4D5E-A804-8C26471E00FA}"/>
+    <workbookView xWindow="1008" yWindow="468" windowWidth="9972" windowHeight="10908" xr2:uid="{8E7FB1D0-DDC4-4D5E-A804-8C26471E00FA}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSheet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>A1 Cell</t>
   </si>
@@ -49,25 +49,34 @@
     <t>A2</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
     <t>C3</t>
   </si>
   <si>
-    <t>B3</t>
+    <t>This is just a test file, leave all sheet names as they are</t>
+  </si>
+  <si>
+    <t>Hello it is two twenty</t>
+  </si>
+  <si>
+    <t>levy</t>
   </si>
   <si>
     <t>A3</t>
   </si>
   <si>
-    <t>This is just a test file, leave all sheet names as they are</t>
-  </si>
-  <si>
-    <t>Hey Dillen its eleven</t>
+    <t>ctc</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21585F4-5811-4635-A800-D557D34F43B8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,26 +452,37 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -480,7 +500,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>